<commit_message>
Premiers pas avec Git - 2023-10-02
</commit_message>
<xml_diff>
--- a/# Facture modèle # 2.xlsx
+++ b/# Facture modèle # 2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC FISCALITÉ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F55C8CA-1379-442B-80E2-6A3C7F06E034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0CCFCE-01AC-4140-9621-0118A6930D0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{804D149D-064E-4534-92B6-566C725D8875}"/>
   </bookViews>
@@ -1219,8 +1219,8 @@
   </sheetPr>
   <dimension ref="A12:F88"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A5" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>